<commit_message>
cập nhật xóa text trong input
</commit_message>
<xml_diff>
--- a/CAP_TEAM05_2022/Uploads/Mau_Nhap_25_05_2023 11_30_31 SA (1).xlsx
+++ b/CAP_TEAM05_2022/Uploads/Mau_Nhap_25_05_2023 11_30_31 SA (1).xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ADMIN\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{62B979EB-03DD-41D3-AB8A-7046F15AC33D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6F5E0268-92DE-4184-A739-B07A5D6219F5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1253,7 +1253,7 @@
   <dimension ref="A1:K144"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A130" workbookViewId="0">
-      <selection activeCell="K142" sqref="K142"/>
+      <selection activeCell="E136" sqref="E136"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="20" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>